<commit_message>
working on main div for content
</commit_message>
<xml_diff>
--- a/Task8-1-ui-challenge.xlsx
+++ b/Task8-1-ui-challenge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive\Documents\CodeTribe\Task8-1-ui-challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05D7BDE8-9173-4935-9E33-DA7A73E463B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFD5905-DDE9-46D2-861D-572E1B385D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ED682E4A-D565-42F6-8A2D-6C96A452CE15}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Backlog</t>
   </si>
@@ -54,6 +54,36 @@
   </si>
   <si>
     <t>Finished</t>
+  </si>
+  <si>
+    <t>1. Create Header component</t>
+  </si>
+  <si>
+    <t>2. Create Main component</t>
+  </si>
+  <si>
+    <t>3. Create Footer component</t>
+  </si>
+  <si>
+    <t>4. Create navbar component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Create Buttons component </t>
+  </si>
+  <si>
+    <t>6. Create Heading component</t>
+  </si>
+  <si>
+    <t>7. Create Icons component</t>
+  </si>
+  <si>
+    <t>8. Create Images component</t>
+  </si>
+  <si>
+    <t>✅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. </t>
   </si>
 </sst>
 </file>
@@ -161,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -173,6 +203,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,7 +550,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,72 +584,106 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>

</xml_diff>